<commit_message>
lighting for catheterisation_wmoen scene
</commit_message>
<xml_diff>
--- a/Protocol_preparation Files/Actions_overviews/Action_overview_catheterisation_Women.xlsx
+++ b/Protocol_preparation Files/Actions_overviews/Action_overview_catheterisation_Women.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/triplemotionmedia 1/Documents/Care Up Game/Protocol_preparation Files/Actions_overviews/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Gijs Tempel.000\Documents\care-up\Protocol_preparation Files\Actions_overviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BBDFC1-B5AF-4D96-9E6F-E501B82AFBB0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="124">
   <si>
     <t>Index</t>
   </si>
@@ -351,14 +352,59 @@
     <t>Alexander</t>
   </si>
   <si>
-    <t xml:space="preserve">Creating </t>
+    <t>Creating move positions for GauzeTrayWet &amp; PlasticTrashbucket</t>
+  </si>
+  <si>
+    <t>GauzeTrayWet &amp; PlasticTrashbucket need to be moved within the protocol. To do this, we need multiple drop locations. Please do this for GauzeTrayWet &amp; PlasticTrashbucket. How to do this can be scene here: https://github.com/GijsTempel/care-up/wiki/Objects under title ' moving objects'</t>
+  </si>
+  <si>
+    <t>Implement, medium priority develop</t>
+  </si>
+  <si>
+    <t>Creating holding animation for PlasticTrashbucket</t>
+  </si>
+  <si>
+    <t>In this protocol we need to move the PasticTrashbucket. Please create a holding animaton for this</t>
+  </si>
+  <si>
+    <t>Animation, medium priority develop</t>
+  </si>
+  <si>
+    <t>Vitalii</t>
+  </si>
+  <si>
+    <t>Adding Place Gauze tray  &amp; plastic trashbucket. on pad step to XML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding Place Gauze tray  &amp; plastic trashbucket. on pad to XML actions list. Create to seperate actions for PlasticTrashBucket and GauzeTray so players can move it in custom order. </t>
+  </si>
+  <si>
+    <t>Creating animation sequence for steps (11t/m17)</t>
+  </si>
+  <si>
+    <t>Creating animation sequence for cleaning genitals</t>
+  </si>
+  <si>
+    <t>Implementing holding animation issue #851</t>
+  </si>
+  <si>
+    <t>Implement holding animation of PlasticTrashbucket so it can be called in XML</t>
+  </si>
+  <si>
+    <t>Adding animation sequence steps for cleaning genitals to actions XML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating animations sequence XML for cleaning genitals animation sequence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementing animation sequence so it can be called in XML </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -379,8 +425,15 @@
       <color theme="1"/>
       <name val="Calibri (Hoofdtekst)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +458,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -415,10 +473,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -426,15 +485,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -702,23 +766,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="64.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="64.375" customWidth="1"/>
+    <col min="4" max="4" width="25.375" customWidth="1"/>
+    <col min="5" max="5" width="21.625" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -741,7 +805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -758,7 +822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -775,7 +839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -792,7 +856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -809,7 +873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -826,7 +890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -843,12 +907,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="E8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -865,7 +929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -882,12 +946,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="E11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -900,16 +964,16 @@
       <c r="D12" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="E13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -926,7 +990,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -943,7 +1007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -960,12 +1024,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="E18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -982,7 +1046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -999,7 +1063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1016,7 +1080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1033,7 +1097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1050,7 +1114,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1067,7 +1131,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
@@ -1084,12 +1148,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="E26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1106,12 +1170,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="E28" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1125,7 +1189,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1142,7 +1206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -1159,12 +1223,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="E32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -1181,17 +1245,17 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="E34" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="E35" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -1208,7 +1272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -1225,7 +1289,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>59</v>
       </c>
@@ -1242,12 +1306,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="E39" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -1264,12 +1328,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="E41" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>63</v>
       </c>
@@ -1286,7 +1350,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -1303,7 +1367,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" s="6" t="s">
         <v>64</v>
       </c>
@@ -1320,7 +1384,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" s="6" t="s">
         <v>66</v>
       </c>
@@ -1337,7 +1401,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" s="6" t="s">
         <v>67</v>
       </c>
@@ -1354,7 +1418,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" s="6" t="s">
         <v>68</v>
       </c>
@@ -1371,7 +1435,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" s="6" t="s">
         <v>70</v>
       </c>
@@ -1388,7 +1452,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" s="6" t="s">
         <v>71</v>
       </c>
@@ -1405,7 +1469,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" s="6" t="s">
         <v>73</v>
       </c>
@@ -1422,7 +1486,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" s="6" t="s">
         <v>74</v>
       </c>
@@ -1439,12 +1503,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="E52" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -1461,12 +1525,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="E54" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>77</v>
       </c>
@@ -1483,12 +1547,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="E56" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>78</v>
       </c>
@@ -1505,7 +1569,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>79</v>
       </c>
@@ -1522,7 +1586,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>80</v>
       </c>
@@ -1539,7 +1603,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>83</v>
       </c>
@@ -1556,7 +1620,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>84</v>
       </c>
@@ -1573,7 +1637,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>86</v>
       </c>
@@ -1590,7 +1654,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>89</v>
       </c>
@@ -1607,7 +1671,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5">
       <c r="A64" s="6" t="s">
         <v>91</v>
       </c>
@@ -1624,7 +1688,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65" s="6" t="s">
         <v>94</v>
       </c>
@@ -1647,23 +1711,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="43.1640625" customWidth="1"/>
-    <col min="2" max="2" width="54.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="43.125" customWidth="1"/>
+    <col min="2" max="2" width="54.375" customWidth="1"/>
+    <col min="3" max="3" width="64.375" customWidth="1"/>
+    <col min="4" max="4" width="32.625" customWidth="1"/>
+    <col min="5" max="5" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
@@ -1680,40 +1744,114 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>99</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="3" spans="1:5">
+      <c r="B3" s="7" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="C3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjustements to issue file
</commit_message>
<xml_diff>
--- a/Protocol_preparation Files/Actions_overviews/Action_overview_catheterisation_Women.xlsx
+++ b/Protocol_preparation Files/Actions_overviews/Action_overview_catheterisation_Women.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gast gebruiker\Documents\care-up\Protocol_preparation Files\Actions_overviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0985C8D9-0033-44F8-B288-9242AC75CEF0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D8C4FA23-5BB1-44B8-A15E-B5F38A63E0EF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -912,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1485,10 +1485,10 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="6">
         <v>27</v>
       </c>
       <c r="C42">
@@ -1502,10 +1502,10 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="6">
         <v>28</v>
       </c>
       <c r="C43">
@@ -1519,10 +1519,10 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="6">
         <v>29</v>
       </c>
       <c r="C44">
@@ -1536,10 +1536,10 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="6">
         <v>30</v>
       </c>
       <c r="C45">
@@ -1553,10 +1553,10 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="6">
         <v>31</v>
       </c>
       <c r="C46">
@@ -1570,10 +1570,10 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="6">
         <v>32</v>
       </c>
       <c r="C47">
@@ -1587,10 +1587,10 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="6">
         <v>33</v>
       </c>
       <c r="C48">
@@ -1604,10 +1604,10 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="6">
         <v>34</v>
       </c>
       <c r="C49">
@@ -1621,10 +1621,10 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="6">
         <v>35</v>
       </c>
       <c r="C50">
@@ -1638,10 +1638,10 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="6">
         <v>36</v>
       </c>
       <c r="C51">
@@ -1655,15 +1655,17 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
       <c r="E52" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="6">
         <v>37</v>
       </c>
       <c r="C53">
@@ -1677,15 +1679,17 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
       <c r="E54" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="6">
         <v>38</v>
       </c>
       <c r="C55">
@@ -1699,15 +1703,17 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
       <c r="E56" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="6">
         <v>39</v>
       </c>
       <c r="C57">
@@ -1721,10 +1727,10 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="6">
         <v>40</v>
       </c>
       <c r="C58">
@@ -1738,10 +1744,10 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="6">
         <v>41</v>
       </c>
       <c r="C59">
@@ -1865,8 +1871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C24" sqref="B23:C24"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>